<commit_message>
Analyze the no_vote and only_vote accuracies
</commit_message>
<xml_diff>
--- a/accuracy_data.xlsx
+++ b/accuracy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cococ\Documents\GitHub\LLMafia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372178B-CBFC-4ABA-93D8-E692B69B87AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C652AB1-9656-4CA6-ABB2-CA75DC30215F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F1A58C9-AC47-4229-89D7-F830C065A130}"/>
+    <workbookView xWindow="45" yWindow="3780" windowWidth="24255" windowHeight="15345" xr2:uid="{1F1A58C9-AC47-4229-89D7-F830C065A130}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Bystander</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>Exact Match - Random</t>
+  </si>
+  <si>
+    <t>37.86% (53.57%)</t>
+  </si>
+  <si>
+    <t>38.57% (56%, random 20%, random 33% if LLM is smart)</t>
+  </si>
+  <si>
+    <t>49.29% (47.86%)</t>
+  </si>
+  <si>
+    <t>47.06% (57.35%)</t>
+  </si>
+  <si>
+    <t>Ablation Study: Only Voting Information</t>
+  </si>
+  <si>
+    <t>Ablation Study: Without Voting Information</t>
   </si>
 </sst>
 </file>
@@ -592,16 +610,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B1576-3372-46CE-9865-A0E377F15A62}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
@@ -645,11 +663,11 @@
       <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19">
-        <v>0.38569999999999999</v>
-      </c>
-      <c r="C5" s="19">
-        <v>0.4929</v>
+      <c r="B5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="11"/>
     </row>
@@ -657,11 +675,11 @@
       <c r="A6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19">
-        <v>0.47060000000000002</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0.37859999999999999</v>
+      <c r="B6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="11"/>
     </row>
@@ -737,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="9">
-        <v>0.28570000000000001</v>
+        <v>0.31430000000000002</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -755,10 +773,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="9">
-        <v>0.28570000000000001</v>
+        <v>0.51429999999999998</v>
       </c>
       <c r="D16" s="4">
-        <v>0</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="E16" s="7">
         <v>0.8</v>
@@ -775,16 +793,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="11">
         <v>3</v>
       </c>
       <c r="C17" s="9">
-        <v>0.48570000000000002</v>
+        <v>0.6875</v>
       </c>
       <c r="D17" s="8">
-        <v>8.5699999999999998E-2</v>
+        <v>0.125</v>
       </c>
       <c r="E17" s="7">
         <v>0.75</v>
@@ -801,16 +819,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B18" s="11">
         <v>4</v>
       </c>
       <c r="C18" s="10">
-        <v>0.25</v>
+        <v>0.77780000000000005</v>
       </c>
       <c r="D18" s="4">
-        <v>0</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
@@ -826,108 +844,60 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>32</v>
-      </c>
-      <c r="B19" s="11">
-        <v>5</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0.4375</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
       <c r="G19" s="3"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>32</v>
-      </c>
-      <c r="B20" s="11">
-        <v>6</v>
-      </c>
-      <c r="C20" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0.15620000000000001</v>
-      </c>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>9</v>
-      </c>
-      <c r="B21" s="11">
-        <v>7</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="5"/>
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>9</v>
-      </c>
-      <c r="B22" s="11">
-        <v>8</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0.77780000000000005</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
       <c r="G22" s="5"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
-        <v>9</v>
-      </c>
-      <c r="B23" s="11">
-        <v>9</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0.88890000000000002</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0.22220000000000001</v>
-      </c>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>9</v>
-      </c>
-      <c r="B24" s="11">
-        <v>10</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0.77780000000000005</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0.1111</v>
-      </c>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
@@ -940,11 +910,11 @@
       </c>
       <c r="C25" s="14">
         <f t="shared" ref="C25:H25" si="0">AVERAGE(C16:C18)</f>
-        <v>0.3404666666666667</v>
+        <v>0.65986666666666671</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" si="0"/>
-        <v>2.8566666666666667E-2</v>
+        <v>0.14430000000000001</v>
       </c>
       <c r="E25" s="16">
         <f t="shared" si="0"/>
@@ -966,6 +936,440 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>35</v>
+      </c>
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.62860000000000005</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>35</v>
+      </c>
+      <c r="B32" s="11">
+        <v>2</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11">
+        <v>3</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0.1875</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>9</v>
+      </c>
+      <c r="B34" s="11">
+        <v>4</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="H34" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="14">
+        <f t="shared" ref="C41:H41" si="1">AVERAGE(C32:C34)</f>
+        <v>0.67386666666666672</v>
+      </c>
+      <c r="D41" s="15">
+        <f t="shared" si="1"/>
+        <v>8.1533333333333333E-2</v>
+      </c>
+      <c r="E41" s="16">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="F41" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <f t="shared" si="1"/>
+        <v>0.34383333333333338</v>
+      </c>
+      <c r="H41" s="15">
+        <f t="shared" si="1"/>
+        <v>1.8133333333333335E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>35</v>
+      </c>
+      <c r="B45" s="11">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0.37140000000000001</v>
+      </c>
+      <c r="D45" s="4">
+        <v>2.86E-2</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>35</v>
+      </c>
+      <c r="B46" s="11">
+        <v>2</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.4667</v>
+      </c>
+      <c r="F46" s="8">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="H46" s="8">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>32</v>
+      </c>
+      <c r="B47" s="11">
+        <v>3</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.71879999999999999</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="H47" s="8">
+        <v>1.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>9</v>
+      </c>
+      <c r="B48" s="11">
+        <v>4</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0.88890000000000002</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F48" s="8">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="H48" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="14">
+        <f t="shared" ref="C55:H55" si="2">AVERAGE(C46:C48)</f>
+        <v>0.67876666666666663</v>
+      </c>
+      <c r="D55" s="15">
+        <f t="shared" si="2"/>
+        <v>0.18133333333333335</v>
+      </c>
+      <c r="E55" s="16">
+        <f t="shared" si="2"/>
+        <v>0.68333333333333324</v>
+      </c>
+      <c r="F55" s="15">
+        <f t="shared" si="2"/>
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="G55" s="16">
+        <f t="shared" si="2"/>
+        <v>0.34383333333333338</v>
+      </c>
+      <c r="H55" s="15">
+        <f t="shared" si="2"/>
+        <v>1.8133333333333335E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>